<commit_message>
Crop production was linked to the wrong GHG emissions.
</commit_message>
<xml_diff>
--- a/Data/GHG_concordance.xlsx
+++ b/Data/GHG_concordance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxime\PycharmProjects\OpenIOCanada\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7351CB-8F78-4700-9DA3-9832ED18CA1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F1BE3E-0E87-45DB-9F2D-F0179A3712D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22200" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22200" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary level" sheetId="1" r:id="rId1"/>
@@ -1589,7 +1589,7 @@
   <dimension ref="A1:B113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2512,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36540CB5-4DD8-451C-8C6B-5D07C0AD9262}">
   <dimension ref="A1:B113"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2574,12 +2574,12 @@
       <c r="A7" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3429,8 +3429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15253D72-A81D-4E40-B134-6272BB3EBEC1}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3494,19 +3494,19 @@
       <c r="A7" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D7" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -4574,8 +4574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C4EC233-B2C0-4570-A3A0-C38B0FCBFD6E}">
   <dimension ref="A1:N113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4641,22 +4641,22 @@
       <c r="A7" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" t="s">
-        <v>332</v>
-      </c>
-      <c r="E7" t="s">
-        <v>333</v>
-      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" t="s">
+        <v>332</v>
+      </c>
+      <c r="E8" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>